<commit_message>
Chech out updates new
</commit_message>
<xml_diff>
--- a/storage/app/excel/template.xlsx
+++ b/storage/app/excel/template.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1008">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1010">
   <si>
     <t>Zone d'intervention</t>
   </si>
@@ -1546,667 +1546,673 @@
     <t>Bazdouz salah</t>
   </si>
   <si>
-    <t>Non installé</t>
+    <t>Problème</t>
+  </si>
+  <si>
+    <t>Not Appliqué</t>
+  </si>
+  <si>
+    <t>Oui</t>
+  </si>
+  <si>
+    <t>BF06FA3PAG07873</t>
+  </si>
+  <si>
+    <t>BF06FA3PAG9615A</t>
+  </si>
+  <si>
+    <t>AHO-1051</t>
+  </si>
+  <si>
+    <t>AHO-1056</t>
+  </si>
+  <si>
+    <t>BRF-1002</t>
+  </si>
+  <si>
+    <t>IP/WDM</t>
+  </si>
+  <si>
+    <t>BRF-1003</t>
+  </si>
+  <si>
+    <t>BRF-1004</t>
+  </si>
+  <si>
+    <t>BRF-1006</t>
+  </si>
+  <si>
+    <t>BRF-1008</t>
+  </si>
+  <si>
+    <t>BRF-P002</t>
+  </si>
+  <si>
+    <t>BRK-1011</t>
+  </si>
+  <si>
+    <t>DRI-1005</t>
+  </si>
+  <si>
+    <t>ELA-1001</t>
+  </si>
+  <si>
+    <t>IP/SDH</t>
+  </si>
+  <si>
+    <t>FIG-1002</t>
+  </si>
+  <si>
+    <t>FIG-1004</t>
+  </si>
+  <si>
+    <t>FIG-1005</t>
+  </si>
+  <si>
+    <t>GRC-1004</t>
+  </si>
+  <si>
+    <t>GRC-1005</t>
+  </si>
+  <si>
+    <t>GRC-1020</t>
+  </si>
+  <si>
+    <t>JRD-1001</t>
+  </si>
+  <si>
+    <t>JRD-1005</t>
+  </si>
+  <si>
+    <t>KET-1002</t>
+  </si>
+  <si>
+    <t>MSN-1001</t>
+  </si>
+  <si>
+    <t>NAD-1014</t>
+  </si>
+  <si>
+    <t>NAD-1018</t>
+  </si>
+  <si>
+    <t>NAD-1020</t>
+  </si>
+  <si>
+    <t>NAD-1031</t>
+  </si>
+  <si>
+    <t>NAD-1045</t>
+  </si>
+  <si>
+    <t>NAI-1003</t>
+  </si>
+  <si>
+    <t>OUJ-1006</t>
+  </si>
+  <si>
+    <t>OUJ-1018</t>
+  </si>
+  <si>
+    <t>OUJ-1019</t>
+  </si>
+  <si>
+    <t>OUJ-1020</t>
+  </si>
+  <si>
+    <t>TRG-1001</t>
+  </si>
+  <si>
+    <t>TRG-1008</t>
+  </si>
+  <si>
+    <t>ZAK-1007</t>
+  </si>
+  <si>
+    <t>rabat</t>
+  </si>
+  <si>
+    <t>SKI-1011</t>
+  </si>
+  <si>
+    <t>INDOOR</t>
+  </si>
+  <si>
+    <t>MAA-1001</t>
+  </si>
+  <si>
+    <t>MAA-1005</t>
+  </si>
+  <si>
+    <t>GNZ-1002</t>
+  </si>
+  <si>
+    <t>BMA-1006</t>
+  </si>
+  <si>
+    <t>RAB-1041</t>
+  </si>
+  <si>
+    <t>RAB-1301</t>
+  </si>
+  <si>
+    <t>RAB-1065</t>
+  </si>
+  <si>
+    <t>SKI-1004</t>
+  </si>
+  <si>
+    <t>SKI-1015</t>
+  </si>
+  <si>
+    <t>OUTDOOR</t>
+  </si>
+  <si>
+    <t>SKI-1014</t>
+  </si>
+  <si>
+    <t>RAB-1008</t>
+  </si>
+  <si>
+    <t>RAB-1415</t>
+  </si>
+  <si>
+    <t>RAB-1086</t>
+  </si>
+  <si>
+    <t>RAB-1014</t>
+  </si>
+  <si>
+    <t>RAB-1053</t>
+  </si>
+  <si>
+    <t>KEN-1025</t>
+  </si>
+  <si>
+    <t>SEA-1005</t>
+  </si>
+  <si>
+    <t>SEA-1006</t>
+  </si>
+  <si>
+    <t>SEA-1008</t>
+  </si>
+  <si>
+    <t>SEA-1010</t>
+  </si>
+  <si>
+    <t>OUE-1008</t>
+  </si>
+  <si>
+    <t>OUE-1028</t>
+  </si>
+  <si>
+    <t>OUE-1010</t>
+  </si>
+  <si>
+    <t>OUE-1044</t>
+  </si>
+  <si>
+    <t>OUE-1046</t>
+  </si>
+  <si>
+    <t>OUE-1006</t>
+  </si>
+  <si>
+    <t>OUE-1021</t>
+  </si>
+  <si>
+    <t>OUE-1020</t>
+  </si>
+  <si>
+    <t>SEA-1020</t>
+  </si>
+  <si>
+    <t>SEA-1021</t>
+  </si>
+  <si>
+    <t>SSK-1010</t>
+  </si>
+  <si>
+    <t>SSK-1011</t>
+  </si>
+  <si>
+    <t>SSK-1021</t>
+  </si>
+  <si>
+    <t>SSK-1008</t>
+  </si>
+  <si>
+    <t>OUE-1043</t>
+  </si>
+  <si>
+    <t>OUE-1042</t>
+  </si>
+  <si>
+    <t>OUE-1047</t>
+  </si>
+  <si>
+    <t>SSK-1018</t>
+  </si>
+  <si>
+    <t>SEA-1009</t>
+  </si>
+  <si>
+    <t>DGU-1003</t>
+  </si>
+  <si>
+    <t>DGU-1013</t>
+  </si>
+  <si>
+    <t>DGU-1021</t>
+  </si>
+  <si>
+    <t>DGU-1020</t>
+  </si>
+  <si>
+    <t>GNZ-1001</t>
+  </si>
+  <si>
+    <t>GNZ-1003</t>
+  </si>
+  <si>
+    <t>KHE-1014</t>
+  </si>
+  <si>
+    <t>KHE-1012</t>
+  </si>
+  <si>
+    <t>KHE-1011</t>
+  </si>
+  <si>
+    <t>KHE-1013</t>
+  </si>
+  <si>
+    <t>KHE-1028</t>
+  </si>
+  <si>
+    <t>KHE-1009</t>
+  </si>
+  <si>
+    <t>MDA-1001</t>
+  </si>
+  <si>
+    <t>MDA-1002</t>
+  </si>
+  <si>
+    <t>MDA-1003</t>
+  </si>
+  <si>
+    <t>KEN-1053</t>
+  </si>
+  <si>
+    <t>KEN-1059</t>
+  </si>
+  <si>
+    <t>RMM-1009</t>
+  </si>
+  <si>
+    <t>RMM-1001</t>
+  </si>
+  <si>
+    <t>RMM-1002</t>
+  </si>
+  <si>
+    <t>RMM-1010</t>
+  </si>
+  <si>
+    <t>RMM-1007</t>
+  </si>
+  <si>
+    <t>RMM-1003</t>
+  </si>
+  <si>
+    <t>SBT-1006</t>
+  </si>
+  <si>
+    <t>RAB-1091</t>
+  </si>
+  <si>
+    <t>RAB-1296</t>
+  </si>
+  <si>
+    <t>RAB-1297</t>
+  </si>
+  <si>
+    <t>RAB-1502</t>
+  </si>
+  <si>
+    <t>RAB-1299</t>
+  </si>
+  <si>
+    <t>RAB-1708</t>
+  </si>
+  <si>
+    <t>RAB-1710</t>
+  </si>
+  <si>
+    <t>RAB-1505</t>
+  </si>
+  <si>
+    <t>RAB-1022</t>
+  </si>
+  <si>
+    <t>RAB-1049</t>
+  </si>
+  <si>
+    <t>RAB-1050</t>
+  </si>
+  <si>
+    <t>RAB-1295</t>
+  </si>
+  <si>
+    <t>Tanger</t>
+  </si>
+  <si>
+    <t>AHO-1026</t>
+  </si>
+  <si>
+    <t>BBR-1001</t>
+  </si>
+  <si>
+    <t>BBR-1014</t>
+  </si>
+  <si>
+    <t>BNH-1004</t>
+  </si>
+  <si>
+    <t>BRI-1008</t>
+  </si>
+  <si>
+    <t>CHF-1005</t>
+  </si>
+  <si>
+    <t>CHF-1006</t>
+  </si>
+  <si>
+    <t>CHF-1008</t>
+  </si>
+  <si>
+    <t>CHF-1012</t>
+  </si>
+  <si>
+    <t>Fibré FON</t>
+  </si>
+  <si>
+    <t>CHF-1013</t>
+  </si>
+  <si>
+    <t>CHF-1020</t>
+  </si>
+  <si>
+    <t>ODL-1001</t>
+  </si>
+  <si>
+    <t>ODL-1002</t>
+  </si>
+  <si>
+    <t>ODL-1004</t>
+  </si>
+  <si>
+    <t>ODL-1007</t>
+  </si>
+  <si>
+    <t>ODL-1008</t>
+  </si>
+  <si>
+    <t>ODL-1015</t>
+  </si>
+  <si>
+    <t>ODL-1016</t>
+  </si>
+  <si>
+    <t>TET-1016</t>
+  </si>
+  <si>
+    <t>TET-1018</t>
+  </si>
+  <si>
+    <t>TET-1023</t>
+  </si>
+  <si>
+    <t>TET-1026</t>
+  </si>
+  <si>
+    <t>TET-1027</t>
+  </si>
+  <si>
+    <t>TET-1037</t>
+  </si>
+  <si>
+    <t>TET-1042</t>
+  </si>
+  <si>
+    <t>TET-1048</t>
+  </si>
+  <si>
+    <t>TET-1065</t>
+  </si>
+  <si>
+    <t>TET-1074</t>
+  </si>
+  <si>
+    <t>TET-1089</t>
+  </si>
+  <si>
+    <t>TET-1098</t>
+  </si>
+  <si>
+    <t>TET-1109</t>
+  </si>
+  <si>
+    <t>TET-1121</t>
+  </si>
+  <si>
+    <t>TET-1126</t>
+  </si>
+  <si>
+    <t>TET-1136</t>
+  </si>
+  <si>
+    <t>TET-1137</t>
+  </si>
+  <si>
+    <t>TET-1186</t>
+  </si>
+  <si>
+    <t>TET-1191</t>
+  </si>
+  <si>
+    <t>ASI-1004</t>
+  </si>
+  <si>
+    <t>ASI-1006</t>
+  </si>
+  <si>
+    <t>Metro IP</t>
+  </si>
+  <si>
+    <t>ASI-1007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASI-1026 </t>
+  </si>
+  <si>
+    <t>FON</t>
+  </si>
+  <si>
+    <t>LAR-1011</t>
+  </si>
+  <si>
+    <t>LAR-1046</t>
+  </si>
+  <si>
+    <t>MYB-1001</t>
+  </si>
+  <si>
+    <t>CWDM +Métro IP</t>
+  </si>
+  <si>
+    <t>TAN-1010</t>
+  </si>
+  <si>
+    <t>Métro ( Ex WDM)</t>
+  </si>
+  <si>
+    <t>Nok</t>
+  </si>
+  <si>
+    <t>TAN-1019</t>
+  </si>
+  <si>
+    <t>TAN-1038</t>
+  </si>
+  <si>
+    <t>TAN-1050</t>
+  </si>
+  <si>
+    <t>TAN-1051</t>
+  </si>
+  <si>
+    <t>TAN-1068</t>
+  </si>
+  <si>
+    <t>TAN-1124</t>
+  </si>
+  <si>
+    <t>TAN-1128</t>
+  </si>
+  <si>
+    <t>TAN-1161</t>
+  </si>
+  <si>
+    <t>TAN-1230</t>
+  </si>
+  <si>
+    <t>TAN-1323</t>
+  </si>
+  <si>
+    <t>TAN-1360</t>
+  </si>
+  <si>
+    <t>TAN-1396</t>
+  </si>
+  <si>
+    <t>TGS-1002</t>
+  </si>
+  <si>
+    <t>Metro IP ( CWDM installé)</t>
+  </si>
+  <si>
+    <t>TET-1080</t>
+  </si>
+  <si>
+    <t>TET-1052</t>
+  </si>
+  <si>
+    <t>TET-1170</t>
+  </si>
+  <si>
+    <t>CHF-1033</t>
+  </si>
+  <si>
+    <t>TET-1091</t>
+  </si>
+  <si>
+    <t>TET-1280</t>
+  </si>
+  <si>
+    <t>TET-1019</t>
+  </si>
+  <si>
+    <t>TET-1038</t>
+  </si>
+  <si>
+    <t>TET-1084</t>
+  </si>
+  <si>
+    <t>TET-1092</t>
+  </si>
+  <si>
+    <t>TET-1103</t>
+  </si>
+  <si>
+    <t>TET-1149</t>
+  </si>
+  <si>
+    <t>TET-1160</t>
+  </si>
+  <si>
+    <t>TET-1203</t>
+  </si>
+  <si>
+    <t>TAN-1142</t>
+  </si>
+  <si>
+    <t>TAN-1149</t>
+  </si>
+  <si>
+    <t>TAN-1170</t>
+  </si>
+  <si>
+    <t>TAN-1176</t>
+  </si>
+  <si>
+    <t>TAN-1202</t>
+  </si>
+  <si>
+    <t>TAN-1268</t>
+  </si>
+  <si>
+    <t>TAN-1300</t>
+  </si>
+  <si>
+    <t>TAN-1325</t>
+  </si>
+  <si>
+    <t>TAN-1326</t>
+  </si>
+  <si>
+    <t>TET-1172</t>
+  </si>
+  <si>
+    <t>TET-1183</t>
+  </si>
+  <si>
+    <t>TET-1212</t>
+  </si>
+  <si>
+    <t>TET-1214</t>
+  </si>
+  <si>
+    <t>TET-1227</t>
+  </si>
+  <si>
+    <t>TET-1232</t>
+  </si>
+  <si>
+    <t>TET-1241</t>
+  </si>
+  <si>
+    <t>TET-1246</t>
+  </si>
+  <si>
+    <t>TET-1249</t>
+  </si>
+  <si>
+    <t>marrakech</t>
+  </si>
+  <si>
+    <t>MNB-1011</t>
+  </si>
+  <si>
+    <t>Amine chayaoui</t>
   </si>
   <si>
     <t>N/A</t>
   </si>
   <si>
     <t>Installé</t>
-  </si>
-  <si>
-    <t>BF06FA3PAG07873</t>
-  </si>
-  <si>
-    <t>BF06FA3PAG9615A</t>
-  </si>
-  <si>
-    <t>AHO-1051</t>
-  </si>
-  <si>
-    <t>AHO-1056</t>
-  </si>
-  <si>
-    <t>BRF-1002</t>
-  </si>
-  <si>
-    <t>IP/WDM</t>
-  </si>
-  <si>
-    <t>BRF-1003</t>
-  </si>
-  <si>
-    <t>BRF-1004</t>
-  </si>
-  <si>
-    <t>BRF-1006</t>
-  </si>
-  <si>
-    <t>BRF-1008</t>
-  </si>
-  <si>
-    <t>BRF-P002</t>
-  </si>
-  <si>
-    <t>BRK-1011</t>
-  </si>
-  <si>
-    <t>DRI-1005</t>
-  </si>
-  <si>
-    <t>ELA-1001</t>
-  </si>
-  <si>
-    <t>IP/SDH</t>
-  </si>
-  <si>
-    <t>FIG-1002</t>
-  </si>
-  <si>
-    <t>FIG-1004</t>
-  </si>
-  <si>
-    <t>FIG-1005</t>
-  </si>
-  <si>
-    <t>GRC-1004</t>
-  </si>
-  <si>
-    <t>GRC-1005</t>
-  </si>
-  <si>
-    <t>GRC-1020</t>
-  </si>
-  <si>
-    <t>JRD-1001</t>
-  </si>
-  <si>
-    <t>JRD-1005</t>
-  </si>
-  <si>
-    <t>KET-1002</t>
-  </si>
-  <si>
-    <t>MSN-1001</t>
-  </si>
-  <si>
-    <t>NAD-1014</t>
-  </si>
-  <si>
-    <t>NAD-1018</t>
-  </si>
-  <si>
-    <t>NAD-1020</t>
-  </si>
-  <si>
-    <t>NAD-1031</t>
-  </si>
-  <si>
-    <t>NAD-1045</t>
-  </si>
-  <si>
-    <t>NAI-1003</t>
-  </si>
-  <si>
-    <t>OUJ-1006</t>
-  </si>
-  <si>
-    <t>OUJ-1018</t>
-  </si>
-  <si>
-    <t>OUJ-1019</t>
-  </si>
-  <si>
-    <t>OUJ-1020</t>
-  </si>
-  <si>
-    <t>TRG-1001</t>
-  </si>
-  <si>
-    <t>TRG-1008</t>
-  </si>
-  <si>
-    <t>ZAK-1007</t>
-  </si>
-  <si>
-    <t>rabat</t>
-  </si>
-  <si>
-    <t>SKI-1011</t>
-  </si>
-  <si>
-    <t>INDOOR</t>
-  </si>
-  <si>
-    <t>MAA-1001</t>
-  </si>
-  <si>
-    <t>MAA-1005</t>
-  </si>
-  <si>
-    <t>GNZ-1002</t>
-  </si>
-  <si>
-    <t>BMA-1006</t>
-  </si>
-  <si>
-    <t>RAB-1041</t>
-  </si>
-  <si>
-    <t>RAB-1301</t>
-  </si>
-  <si>
-    <t>RAB-1065</t>
-  </si>
-  <si>
-    <t>SKI-1004</t>
-  </si>
-  <si>
-    <t>SKI-1015</t>
-  </si>
-  <si>
-    <t>OUTDOOR</t>
-  </si>
-  <si>
-    <t>SKI-1014</t>
-  </si>
-  <si>
-    <t>RAB-1008</t>
-  </si>
-  <si>
-    <t>RAB-1415</t>
-  </si>
-  <si>
-    <t>RAB-1086</t>
-  </si>
-  <si>
-    <t>RAB-1014</t>
-  </si>
-  <si>
-    <t>RAB-1053</t>
-  </si>
-  <si>
-    <t>KEN-1025</t>
-  </si>
-  <si>
-    <t>SEA-1005</t>
-  </si>
-  <si>
-    <t>SEA-1006</t>
-  </si>
-  <si>
-    <t>SEA-1008</t>
-  </si>
-  <si>
-    <t>SEA-1010</t>
-  </si>
-  <si>
-    <t>OUE-1008</t>
-  </si>
-  <si>
-    <t>OUE-1028</t>
-  </si>
-  <si>
-    <t>OUE-1010</t>
-  </si>
-  <si>
-    <t>OUE-1044</t>
-  </si>
-  <si>
-    <t>OUE-1046</t>
-  </si>
-  <si>
-    <t>OUE-1006</t>
-  </si>
-  <si>
-    <t>OUE-1021</t>
-  </si>
-  <si>
-    <t>OUE-1020</t>
-  </si>
-  <si>
-    <t>SEA-1020</t>
-  </si>
-  <si>
-    <t>SEA-1021</t>
-  </si>
-  <si>
-    <t>SSK-1010</t>
-  </si>
-  <si>
-    <t>SSK-1011</t>
-  </si>
-  <si>
-    <t>SSK-1021</t>
-  </si>
-  <si>
-    <t>SSK-1008</t>
-  </si>
-  <si>
-    <t>OUE-1043</t>
-  </si>
-  <si>
-    <t>OUE-1042</t>
-  </si>
-  <si>
-    <t>OUE-1047</t>
-  </si>
-  <si>
-    <t>SSK-1018</t>
-  </si>
-  <si>
-    <t>SEA-1009</t>
-  </si>
-  <si>
-    <t>DGU-1003</t>
-  </si>
-  <si>
-    <t>DGU-1013</t>
-  </si>
-  <si>
-    <t>DGU-1021</t>
-  </si>
-  <si>
-    <t>DGU-1020</t>
-  </si>
-  <si>
-    <t>GNZ-1001</t>
-  </si>
-  <si>
-    <t>GNZ-1003</t>
-  </si>
-  <si>
-    <t>KHE-1014</t>
-  </si>
-  <si>
-    <t>KHE-1012</t>
-  </si>
-  <si>
-    <t>KHE-1011</t>
-  </si>
-  <si>
-    <t>KHE-1013</t>
-  </si>
-  <si>
-    <t>KHE-1028</t>
-  </si>
-  <si>
-    <t>KHE-1009</t>
-  </si>
-  <si>
-    <t>MDA-1001</t>
-  </si>
-  <si>
-    <t>MDA-1002</t>
-  </si>
-  <si>
-    <t>MDA-1003</t>
-  </si>
-  <si>
-    <t>KEN-1053</t>
-  </si>
-  <si>
-    <t>KEN-1059</t>
-  </si>
-  <si>
-    <t>RMM-1009</t>
-  </si>
-  <si>
-    <t>RMM-1001</t>
-  </si>
-  <si>
-    <t>RMM-1002</t>
-  </si>
-  <si>
-    <t>RMM-1010</t>
-  </si>
-  <si>
-    <t>RMM-1007</t>
-  </si>
-  <si>
-    <t>RMM-1003</t>
-  </si>
-  <si>
-    <t>SBT-1006</t>
-  </si>
-  <si>
-    <t>RAB-1091</t>
-  </si>
-  <si>
-    <t>RAB-1296</t>
-  </si>
-  <si>
-    <t>RAB-1297</t>
-  </si>
-  <si>
-    <t>RAB-1502</t>
-  </si>
-  <si>
-    <t>RAB-1299</t>
-  </si>
-  <si>
-    <t>RAB-1708</t>
-  </si>
-  <si>
-    <t>RAB-1710</t>
-  </si>
-  <si>
-    <t>RAB-1505</t>
-  </si>
-  <si>
-    <t>RAB-1022</t>
-  </si>
-  <si>
-    <t>RAB-1049</t>
-  </si>
-  <si>
-    <t>RAB-1050</t>
-  </si>
-  <si>
-    <t>RAB-1295</t>
-  </si>
-  <si>
-    <t>Tanger</t>
-  </si>
-  <si>
-    <t>AHO-1026</t>
-  </si>
-  <si>
-    <t>BBR-1001</t>
-  </si>
-  <si>
-    <t>BBR-1014</t>
-  </si>
-  <si>
-    <t>BNH-1004</t>
-  </si>
-  <si>
-    <t>BRI-1008</t>
-  </si>
-  <si>
-    <t>CHF-1005</t>
-  </si>
-  <si>
-    <t>CHF-1006</t>
-  </si>
-  <si>
-    <t>CHF-1008</t>
-  </si>
-  <si>
-    <t>CHF-1012</t>
-  </si>
-  <si>
-    <t>Fibré FON</t>
-  </si>
-  <si>
-    <t>CHF-1013</t>
-  </si>
-  <si>
-    <t>CHF-1020</t>
-  </si>
-  <si>
-    <t>ODL-1001</t>
-  </si>
-  <si>
-    <t>ODL-1002</t>
-  </si>
-  <si>
-    <t>ODL-1004</t>
-  </si>
-  <si>
-    <t>ODL-1007</t>
-  </si>
-  <si>
-    <t>ODL-1008</t>
-  </si>
-  <si>
-    <t>ODL-1015</t>
-  </si>
-  <si>
-    <t>ODL-1016</t>
-  </si>
-  <si>
-    <t>TET-1016</t>
-  </si>
-  <si>
-    <t>TET-1018</t>
-  </si>
-  <si>
-    <t>TET-1023</t>
-  </si>
-  <si>
-    <t>TET-1026</t>
-  </si>
-  <si>
-    <t>TET-1027</t>
-  </si>
-  <si>
-    <t>TET-1037</t>
-  </si>
-  <si>
-    <t>TET-1042</t>
-  </si>
-  <si>
-    <t>TET-1048</t>
-  </si>
-  <si>
-    <t>TET-1065</t>
-  </si>
-  <si>
-    <t>TET-1074</t>
-  </si>
-  <si>
-    <t>TET-1089</t>
-  </si>
-  <si>
-    <t>TET-1098</t>
-  </si>
-  <si>
-    <t>TET-1109</t>
-  </si>
-  <si>
-    <t>TET-1121</t>
-  </si>
-  <si>
-    <t>TET-1126</t>
-  </si>
-  <si>
-    <t>TET-1136</t>
-  </si>
-  <si>
-    <t>TET-1137</t>
-  </si>
-  <si>
-    <t>TET-1186</t>
-  </si>
-  <si>
-    <t>TET-1191</t>
-  </si>
-  <si>
-    <t>ASI-1004</t>
-  </si>
-  <si>
-    <t>ASI-1006</t>
-  </si>
-  <si>
-    <t>Metro IP</t>
-  </si>
-  <si>
-    <t>ASI-1007</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ASI-1026 </t>
-  </si>
-  <si>
-    <t>FON</t>
-  </si>
-  <si>
-    <t>LAR-1011</t>
-  </si>
-  <si>
-    <t>LAR-1046</t>
-  </si>
-  <si>
-    <t>MYB-1001</t>
-  </si>
-  <si>
-    <t>CWDM +Métro IP</t>
-  </si>
-  <si>
-    <t>TAN-1010</t>
-  </si>
-  <si>
-    <t>Métro ( Ex WDM)</t>
-  </si>
-  <si>
-    <t>Nok</t>
-  </si>
-  <si>
-    <t>TAN-1019</t>
-  </si>
-  <si>
-    <t>TAN-1038</t>
-  </si>
-  <si>
-    <t>TAN-1050</t>
-  </si>
-  <si>
-    <t>TAN-1051</t>
-  </si>
-  <si>
-    <t>TAN-1068</t>
-  </si>
-  <si>
-    <t>TAN-1124</t>
-  </si>
-  <si>
-    <t>TAN-1128</t>
-  </si>
-  <si>
-    <t>TAN-1161</t>
-  </si>
-  <si>
-    <t>TAN-1230</t>
-  </si>
-  <si>
-    <t>TAN-1323</t>
-  </si>
-  <si>
-    <t>TAN-1360</t>
-  </si>
-  <si>
-    <t>TAN-1396</t>
-  </si>
-  <si>
-    <t>TGS-1002</t>
-  </si>
-  <si>
-    <t>Metro IP ( CWDM installé)</t>
-  </si>
-  <si>
-    <t>TET-1080</t>
-  </si>
-  <si>
-    <t>TET-1052</t>
-  </si>
-  <si>
-    <t>TET-1170</t>
-  </si>
-  <si>
-    <t>CHF-1033</t>
-  </si>
-  <si>
-    <t>TET-1091</t>
-  </si>
-  <si>
-    <t>TET-1280</t>
-  </si>
-  <si>
-    <t>TET-1019</t>
-  </si>
-  <si>
-    <t>TET-1038</t>
-  </si>
-  <si>
-    <t>TET-1084</t>
-  </si>
-  <si>
-    <t>TET-1092</t>
-  </si>
-  <si>
-    <t>TET-1103</t>
-  </si>
-  <si>
-    <t>TET-1149</t>
-  </si>
-  <si>
-    <t>TET-1160</t>
-  </si>
-  <si>
-    <t>TET-1203</t>
-  </si>
-  <si>
-    <t>TAN-1142</t>
-  </si>
-  <si>
-    <t>TAN-1149</t>
-  </si>
-  <si>
-    <t>TAN-1170</t>
-  </si>
-  <si>
-    <t>TAN-1176</t>
-  </si>
-  <si>
-    <t>TAN-1202</t>
-  </si>
-  <si>
-    <t>TAN-1268</t>
-  </si>
-  <si>
-    <t>TAN-1300</t>
-  </si>
-  <si>
-    <t>TAN-1325</t>
-  </si>
-  <si>
-    <t>TAN-1326</t>
-  </si>
-  <si>
-    <t>TET-1172</t>
-  </si>
-  <si>
-    <t>TET-1183</t>
-  </si>
-  <si>
-    <t>TET-1212</t>
-  </si>
-  <si>
-    <t>TET-1214</t>
-  </si>
-  <si>
-    <t>TET-1227</t>
-  </si>
-  <si>
-    <t>TET-1232</t>
-  </si>
-  <si>
-    <t>TET-1241</t>
-  </si>
-  <si>
-    <t>TET-1246</t>
-  </si>
-  <si>
-    <t>TET-1249</t>
-  </si>
-  <si>
-    <t>marrakech</t>
-  </si>
-  <si>
-    <t>MNB-1011</t>
-  </si>
-  <si>
-    <t>Amine chayaoui</t>
   </si>
   <si>
     <t>BF06FA3PAGC5AB7</t>
@@ -36726,60 +36732,60 @@
         <v>727</v>
       </c>
       <c r="I653" s="10" t="s">
-        <v>508</v>
+        <v>728</v>
       </c>
       <c r="J653" s="10" t="s">
-        <v>508</v>
+        <v>728</v>
       </c>
       <c r="K653" s="10"/>
       <c r="L653" s="10" t="s">
-        <v>508</v>
+        <v>728</v>
       </c>
       <c r="M653" s="10" t="s">
-        <v>508</v>
+        <v>728</v>
       </c>
       <c r="N653" s="10" t="s">
-        <v>508</v>
+        <v>728</v>
       </c>
       <c r="O653" s="10" t="s">
-        <v>509</v>
+        <v>729</v>
       </c>
       <c r="Q653" s="10" t="s">
-        <v>509</v>
+        <v>729</v>
       </c>
       <c r="R653" s="10" t="s">
+        <v>730</v>
+      </c>
+      <c r="S653" s="10" t="s">
         <v>728</v>
-      </c>
-      <c r="S653" s="10" t="s">
-        <v>508</v>
       </c>
       <c r="T653" s="10"/>
       <c r="V653" s="10" t="s">
-        <v>509</v>
+        <v>729</v>
       </c>
       <c r="W653" s="10" t="s">
-        <v>508</v>
+        <v>728</v>
       </c>
       <c r="X653" s="10" t="s">
-        <v>509</v>
+        <v>729</v>
       </c>
       <c r="Y653" s="10" t="s">
-        <v>509</v>
+        <v>729</v>
       </c>
       <c r="Z653" s="10" t="s">
-        <v>509</v>
+        <v>729</v>
       </c>
       <c r="AA653" s="10" t="s">
-        <v>509</v>
+        <v>729</v>
       </c>
       <c r="AB653" s="10" t="s">
-        <v>509</v>
+        <v>729</v>
       </c>
       <c r="AC653" s="10" t="s">
-        <v>509</v>
+        <v>729</v>
       </c>
       <c r="AD653" s="10" t="s">
-        <v>509</v>
+        <v>729</v>
       </c>
       <c r="AE653" s="10" t="s">
         <v>40</v>
@@ -36937,22 +36943,22 @@
     </row>
     <row r="2" spans="1:22" customHeight="1" ht="27">
       <c r="A2" s="16" t="s">
-        <v>729</v>
+        <v>731</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>731</v>
+        <v>733</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>732</v>
+        <v>734</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>733</v>
+        <v>735</v>
       </c>
       <c r="G2" s="19" t="s">
-        <v>734</v>
+        <v>736</v>
       </c>
     </row>
     <row r="3" spans="1:22" customHeight="1" ht="24">
@@ -36981,7 +36987,7 @@
         <v>3</v>
       </c>
       <c r="G5" s="21" t="s">
-        <v>735</v>
+        <v>737</v>
       </c>
     </row>
     <row r="6" spans="1:22">
@@ -36992,7 +36998,7 @@
     </row>
     <row r="8" spans="1:22">
       <c r="A8" s="22" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="B8" s="17" t="str">
         <f>+IF($F$1=1,"Greenfield",IF($F$1=2,"Esthétique",""))</f>
@@ -37002,7 +37008,7 @@
     <row r="9" spans="1:22" customHeight="1" ht="15"/>
     <row r="10" spans="1:22" customHeight="1" ht="24.75">
       <c r="B10" s="145" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c r="C10" s="146"/>
       <c r="D10" s="146"/>
@@ -37011,7 +37017,7 @@
       <c r="G10" s="146"/>
       <c r="H10" s="146"/>
       <c r="I10" s="145" t="s">
-        <v>738</v>
+        <v>740</v>
       </c>
       <c r="J10" s="146"/>
       <c r="K10" s="146"/>
@@ -37021,70 +37027,70 @@
     </row>
     <row r="11" spans="1:22" customHeight="1" ht="46.5" s="11" customFormat="1">
       <c r="A11" s="46" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>740</v>
+        <v>742</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>741</v>
+        <v>743</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>742</v>
+        <v>744</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>743</v>
+        <v>745</v>
       </c>
       <c r="F11" s="25" t="s">
-        <v>744</v>
+        <v>746</v>
       </c>
       <c r="G11" s="25" t="s">
-        <v>745</v>
+        <v>747</v>
       </c>
       <c r="H11" s="29" t="s">
-        <v>746</v>
+        <v>748</v>
       </c>
       <c r="I11" s="26" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
       <c r="J11" s="25" t="s">
-        <v>748</v>
+        <v>750</v>
       </c>
       <c r="K11" s="25" t="s">
-        <v>749</v>
+        <v>751</v>
       </c>
       <c r="L11" s="25" t="s">
-        <v>750</v>
+        <v>752</v>
       </c>
       <c r="M11" s="25" t="s">
-        <v>751</v>
+        <v>753</v>
       </c>
       <c r="N11" s="29" t="s">
-        <v>752</v>
+        <v>754</v>
       </c>
       <c r="O11" s="63" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
       <c r="P11" s="64" t="s">
-        <v>754</v>
+        <v>756</v>
       </c>
       <c r="Q11" s="64" t="s">
-        <v>755</v>
+        <v>757</v>
       </c>
       <c r="R11" s="64" t="s">
-        <v>756</v>
+        <v>758</v>
       </c>
       <c r="S11" s="64" t="s">
-        <v>757</v>
+        <v>759</v>
       </c>
       <c r="T11" s="64" t="s">
-        <v>758</v>
+        <v>760</v>
       </c>
       <c r="U11" s="64" t="s">
-        <v>759</v>
+        <v>761</v>
       </c>
       <c r="V11" s="65" t="s">
-        <v>760</v>
+        <v>762</v>
       </c>
     </row>
     <row r="12" spans="1:22" customHeight="1" ht="21.75">
@@ -37356,7 +37362,7 @@
     </row>
     <row r="15" spans="1:22" customHeight="1" ht="21.75">
       <c r="A15" s="37" t="s">
-        <v>761</v>
+        <v>763</v>
       </c>
       <c r="B15" s="23">
         <f>IF($B$8="",_xlfn.COUNTIFS('Données-Globales'!$A:$A,'Traitement TDB'!$A15),_xlfn.COUNTIFS('Données-Globales'!$A:$A,'Traitement TDB'!$A15,'Données-Globales'!$D:$D,'Traitement TDB'!$B$8))</f>
@@ -37445,7 +37451,7 @@
     </row>
     <row r="16" spans="1:22" customHeight="1" ht="21.75">
       <c r="A16" s="37" t="s">
-        <v>762</v>
+        <v>764</v>
       </c>
       <c r="B16" s="23">
         <f>IF($B$8="",_xlfn.COUNTIFS('Données-Globales'!$A:$A,'Traitement TDB'!$A16),_xlfn.COUNTIFS('Données-Globales'!$A:$A,'Traitement TDB'!$A16,'Données-Globales'!$D:$D,'Traitement TDB'!$B$8))</f>
@@ -37534,7 +37540,7 @@
     </row>
     <row r="17" spans="1:22" customHeight="1" ht="21.75">
       <c r="A17" s="37" t="s">
-        <v>763</v>
+        <v>765</v>
       </c>
       <c r="B17" s="23">
         <f>IF($B$8="",_xlfn.COUNTIFS('Données-Globales'!$A:$A,'Traitement TDB'!$A17),_xlfn.COUNTIFS('Données-Globales'!$A:$A,'Traitement TDB'!$A17,'Données-Globales'!$D:$D,'Traitement TDB'!$B$8))</f>
@@ -37623,7 +37629,7 @@
     </row>
     <row r="18" spans="1:22" customHeight="1" ht="21.75">
       <c r="A18" s="37" t="s">
-        <v>764</v>
+        <v>766</v>
       </c>
       <c r="B18" s="23">
         <f>IF($B$8="",_xlfn.COUNTIFS('Données-Globales'!$A:$A,'Traitement TDB'!$A18),_xlfn.COUNTIFS('Données-Globales'!$A:$A,'Traitement TDB'!$A18,'Données-Globales'!$D:$D,'Traitement TDB'!$B$8))</f>
@@ -37713,7 +37719,7 @@
     <row r="20" spans="1:22" customHeight="1" ht="15"/>
     <row r="21" spans="1:22" customHeight="1" ht="19">
       <c r="B21" s="145" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c r="C21" s="146"/>
       <c r="D21" s="146"/>
@@ -37722,7 +37728,7 @@
       <c r="G21" s="146"/>
       <c r="H21" s="146"/>
       <c r="I21" s="145" t="s">
-        <v>738</v>
+        <v>740</v>
       </c>
       <c r="J21" s="146"/>
       <c r="K21" s="146"/>
@@ -37730,7 +37736,7 @@
       <c r="M21" s="146"/>
       <c r="N21" s="147"/>
       <c r="O21" s="148" t="s">
-        <v>765</v>
+        <v>767</v>
       </c>
       <c r="P21" s="149"/>
       <c r="Q21" s="149"/>
@@ -37742,75 +37748,75 @@
     </row>
     <row r="22" spans="1:22" customHeight="1" ht="87.5">
       <c r="A22" s="67" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="B22" s="68" t="s">
-        <v>740</v>
+        <v>742</v>
       </c>
       <c r="C22" s="69" t="s">
-        <v>741</v>
+        <v>743</v>
       </c>
       <c r="D22" s="69" t="s">
-        <v>742</v>
+        <v>744</v>
       </c>
       <c r="E22" s="69" t="s">
-        <v>743</v>
+        <v>745</v>
       </c>
       <c r="F22" s="69" t="s">
-        <v>744</v>
+        <v>746</v>
       </c>
       <c r="G22" s="69" t="s">
-        <v>745</v>
+        <v>747</v>
       </c>
       <c r="H22" s="70" t="s">
-        <v>746</v>
+        <v>748</v>
       </c>
       <c r="I22" s="71" t="s">
-        <v>766</v>
+        <v>768</v>
       </c>
       <c r="J22" s="69" t="s">
-        <v>767</v>
+        <v>769</v>
       </c>
       <c r="K22" s="69" t="s">
-        <v>768</v>
+        <v>770</v>
       </c>
       <c r="L22" s="69" t="s">
-        <v>769</v>
+        <v>771</v>
       </c>
       <c r="M22" s="69" t="s">
-        <v>770</v>
+        <v>772</v>
       </c>
       <c r="N22" s="70" t="s">
-        <v>771</v>
+        <v>773</v>
       </c>
       <c r="O22" s="66" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
       <c r="P22" s="66" t="s">
-        <v>754</v>
+        <v>756</v>
       </c>
       <c r="Q22" s="66" t="s">
-        <v>755</v>
+        <v>757</v>
       </c>
       <c r="R22" s="66" t="s">
-        <v>756</v>
+        <v>758</v>
       </c>
       <c r="S22" s="66" t="s">
-        <v>757</v>
+        <v>759</v>
       </c>
       <c r="T22" s="66" t="s">
-        <v>758</v>
+        <v>760</v>
       </c>
       <c r="U22" s="66" t="s">
-        <v>759</v>
+        <v>761</v>
       </c>
       <c r="V22" s="66" t="s">
-        <v>760</v>
+        <v>762</v>
       </c>
     </row>
     <row r="23" spans="1:22" customHeight="1" ht="18.5">
       <c r="A23" s="39" t="s">
-        <v>772</v>
+        <v>774</v>
       </c>
       <c r="B23" s="40">
         <f>+SUBTOTAL(9,B12:B18)</f>
@@ -37997,16 +38003,16 @@
   <sheetData>
     <row r="2" spans="1:17">
       <c r="A2" s="16" t="s">
-        <v>729</v>
+        <v>731</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>731</v>
+        <v>733</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>732</v>
+        <v>734</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -38017,7 +38023,7 @@
     </row>
     <row r="5" spans="1:17" customHeight="1" ht="15.5">
       <c r="A5" s="22" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="B5" s="94" t="s">
         <v>38</v>
@@ -38030,7 +38036,7 @@
     <row r="7" spans="1:17" customHeight="1" ht="15"/>
     <row r="8" spans="1:17" customHeight="1" ht="19">
       <c r="B8" s="151" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c r="C8" s="152"/>
       <c r="D8" s="152"/>
@@ -38039,7 +38045,7 @@
       <c r="G8" s="152"/>
       <c r="H8" s="152"/>
       <c r="I8" s="151" t="s">
-        <v>738</v>
+        <v>740</v>
       </c>
       <c r="J8" s="152"/>
       <c r="K8" s="152"/>
@@ -38049,46 +38055,46 @@
     </row>
     <row r="9" spans="1:17" customHeight="1" ht="29.5" s="11" customFormat="1">
       <c r="A9" s="73" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="B9" s="92" t="s">
-        <v>740</v>
+        <v>742</v>
       </c>
       <c r="C9" s="76" t="s">
-        <v>741</v>
+        <v>743</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>742</v>
+        <v>744</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>743</v>
+        <v>745</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>744</v>
+        <v>746</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>745</v>
+        <v>747</v>
       </c>
       <c r="H9" s="74" t="s">
-        <v>746</v>
+        <v>748</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>748</v>
+        <v>750</v>
       </c>
       <c r="K9" s="13" t="s">
-        <v>749</v>
+        <v>751</v>
       </c>
       <c r="L9" s="13" t="s">
-        <v>750</v>
+        <v>752</v>
       </c>
       <c r="M9" s="13" t="s">
-        <v>751</v>
+        <v>753</v>
       </c>
       <c r="N9" s="75" t="s">
-        <v>752</v>
+        <v>754</v>
       </c>
       <c r="O9" s="15"/>
     </row>
@@ -38266,7 +38272,7 @@
     </row>
     <row r="13" spans="1:17">
       <c r="A13" s="78" t="s">
-        <v>761</v>
+        <v>763</v>
       </c>
       <c r="B13" s="80">
         <f>IF($B$5="",_xlfn.COUNTIFS('Données-Globales'!$A:$A,Synthèse!$A13),_xlfn.COUNTIFS('Données-Globales'!$A:$A,Synthèse!$A13,'Données-Globales'!$D:$D,Synthèse!$B$5))</f>
@@ -38323,7 +38329,7 @@
     </row>
     <row r="14" spans="1:17">
       <c r="A14" s="78" t="s">
-        <v>762</v>
+        <v>764</v>
       </c>
       <c r="B14" s="80">
         <f>IF($B$5="",_xlfn.COUNTIFS('Données-Globales'!$A:$A,Synthèse!$A14),_xlfn.COUNTIFS('Données-Globales'!$A:$A,Synthèse!$A14,'Données-Globales'!$D:$D,Synthèse!$B$5))</f>
@@ -38380,7 +38386,7 @@
     </row>
     <row r="15" spans="1:17">
       <c r="A15" s="78" t="s">
-        <v>763</v>
+        <v>765</v>
       </c>
       <c r="B15" s="80">
         <f>IF($B$5="",_xlfn.COUNTIFS('Données-Globales'!$A:$A,Synthèse!$A15),_xlfn.COUNTIFS('Données-Globales'!$A:$A,Synthèse!$A15,'Données-Globales'!$D:$D,Synthèse!$B$5))</f>
@@ -38437,7 +38443,7 @@
     </row>
     <row r="16" spans="1:17" customHeight="1" ht="15">
       <c r="A16" s="78" t="s">
-        <v>764</v>
+        <v>766</v>
       </c>
       <c r="B16" s="80">
         <f>IF($B$5="",_xlfn.COUNTIFS('Données-Globales'!$A:$A,Synthèse!$A16),_xlfn.COUNTIFS('Données-Globales'!$A:$A,Synthèse!$A16,'Données-Globales'!$D:$D,Synthèse!$B$5))</f>
@@ -38494,7 +38500,7 @@
     </row>
     <row r="17" spans="1:17" customHeight="1" ht="19">
       <c r="A17" s="79" t="s">
-        <v>772</v>
+        <v>774</v>
       </c>
       <c r="B17" s="93">
         <f>SUM(B10:B16)</f>
@@ -38552,31 +38558,31 @@
     <row r="20" spans="1:17" customHeight="1" ht="15"/>
     <row r="21" spans="1:17" customHeight="1" ht="62.5" s="11" customFormat="1">
       <c r="A21" s="85" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="B21" s="86" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
       <c r="C21" s="87" t="s">
-        <v>754</v>
+        <v>756</v>
       </c>
       <c r="D21" s="87" t="s">
-        <v>755</v>
+        <v>757</v>
       </c>
       <c r="E21" s="87" t="s">
-        <v>756</v>
+        <v>758</v>
       </c>
       <c r="F21" s="87" t="s">
-        <v>757</v>
+        <v>759</v>
       </c>
       <c r="G21" s="87" t="s">
-        <v>758</v>
+        <v>760</v>
       </c>
       <c r="H21" s="87" t="s">
-        <v>759</v>
+        <v>761</v>
       </c>
       <c r="I21" s="88" t="s">
-        <v>760</v>
+        <v>762</v>
       </c>
       <c r="J21" s="15"/>
       <c r="K21" s="15"/>
@@ -38699,7 +38705,7 @@
     </row>
     <row r="25" spans="1:17">
       <c r="A25" s="51" t="s">
-        <v>761</v>
+        <v>763</v>
       </c>
       <c r="B25" s="54">
         <f>IF($B$5="",_xlfn.COUNTIFS('Données-Globales'!$A:$A,Synthèse!$A25,'Données-Globales'!$I:$I,$A$2),_xlfn.COUNTIFS('Données-Globales'!$A:$A,Synthèse!$A25,'Données-Globales'!$I:$I,$A$2,'Données-Globales'!$D:$D,Synthèse!$B$5))</f>
@@ -38736,7 +38742,7 @@
     </row>
     <row r="26" spans="1:17">
       <c r="A26" s="51" t="s">
-        <v>762</v>
+        <v>764</v>
       </c>
       <c r="B26" s="54">
         <f>IF($B$5="",_xlfn.COUNTIFS('Données-Globales'!$A:$A,Synthèse!$A26,'Données-Globales'!$I:$I,$A$2),_xlfn.COUNTIFS('Données-Globales'!$A:$A,Synthèse!$A26,'Données-Globales'!$I:$I,$A$2,'Données-Globales'!$D:$D,Synthèse!$B$5))</f>
@@ -38773,7 +38779,7 @@
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="51" t="s">
-        <v>763</v>
+        <v>765</v>
       </c>
       <c r="B27" s="54">
         <f>IF($B$5="",_xlfn.COUNTIFS('Données-Globales'!$A:$A,Synthèse!$A27,'Données-Globales'!$I:$I,$A$2),_xlfn.COUNTIFS('Données-Globales'!$A:$A,Synthèse!$A27,'Données-Globales'!$I:$I,$A$2,'Données-Globales'!$D:$D,Synthèse!$B$5))</f>
@@ -38810,7 +38816,7 @@
     </row>
     <row r="28" spans="1:17" customHeight="1" ht="15">
       <c r="A28" s="51" t="s">
-        <v>764</v>
+        <v>766</v>
       </c>
       <c r="B28" s="54">
         <f>IF($B$5="",_xlfn.COUNTIFS('Données-Globales'!$A:$A,Synthèse!$A28,'Données-Globales'!$I:$I,$A$2),_xlfn.COUNTIFS('Données-Globales'!$A:$A,Synthèse!$A28,'Données-Globales'!$I:$I,$A$2,'Données-Globales'!$D:$D,Synthèse!$B$5))</f>
@@ -38847,7 +38853,7 @@
     </row>
     <row r="29" spans="1:17" customHeight="1" ht="19">
       <c r="A29" s="52" t="s">
-        <v>772</v>
+        <v>774</v>
       </c>
       <c r="B29" s="89">
         <f>SUM(B22:B28)</f>
@@ -38925,7 +38931,7 @@
     <row r="1" spans="1:18" customHeight="1" ht="29.5">
       <c r="B1" s="34"/>
       <c r="C1" s="139" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
       <c r="D1" s="139"/>
       <c r="E1" s="139"/>
@@ -38971,7 +38977,7 @@
       <c r="G3" s="36"/>
       <c r="H3" s="36"/>
       <c r="I3" s="140" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="J3" s="140"/>
       <c r="K3" s="140"/>
@@ -38995,7 +39001,7 @@
       <c r="G4" s="36"/>
       <c r="H4" s="36"/>
       <c r="I4" s="140" t="s">
-        <v>775</v>
+        <v>777</v>
       </c>
       <c r="J4" s="140"/>
       <c r="K4" s="140"/>
@@ -39019,7 +39025,7 @@
       <c r="G5" s="36"/>
       <c r="H5" s="36"/>
       <c r="I5" s="141" t="s">
-        <v>776</v>
+        <v>778</v>
       </c>
       <c r="J5" s="141"/>
       <c r="K5" s="141"/>
@@ -39043,7 +39049,7 @@
       <c r="G6" s="36"/>
       <c r="H6" s="36"/>
       <c r="I6" s="140" t="s">
-        <v>777</v>
+        <v>779</v>
       </c>
       <c r="J6" s="140"/>
       <c r="K6" s="140"/>
@@ -39759,16 +39765,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>778</v>
+        <v>780</v>
       </c>
       <c r="B1" t="s">
-        <v>779</v>
+        <v>781</v>
       </c>
       <c r="C1" t="s">
-        <v>780</v>
+        <v>782</v>
       </c>
       <c r="D1" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -39776,7 +39782,7 @@
         <v>37</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>782</v>
+        <v>784</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>0</v>
@@ -39791,7 +39797,7 @@
         <v>91</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>1</v>
@@ -39829,7 +39835,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="9" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="9" t="s">
@@ -39842,7 +39848,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="9" t="s">
-        <v>785</v>
+        <v>787</v>
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="9" t="s">
@@ -39855,10 +39861,10 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="9" t="s">
-        <v>786</v>
+        <v>788</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>787</v>
+        <v>789</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>6</v>
@@ -39870,7 +39876,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="9" t="s">
-        <v>788</v>
+        <v>790</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="9" t="s">
@@ -39883,10 +39889,10 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="9" t="s">
-        <v>789</v>
+        <v>791</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>790</v>
+        <v>792</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>8</v>
@@ -39898,10 +39904,10 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="9" t="s">
-        <v>791</v>
+        <v>793</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>792</v>
+        <v>794</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>9</v>
@@ -39913,10 +39919,10 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="9" t="s">
-        <v>793</v>
+        <v>795</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>794</v>
+        <v>796</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>10</v>
@@ -39928,10 +39934,10 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="9" t="s">
-        <v>795</v>
+        <v>797</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>11</v>
@@ -39943,10 +39949,10 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="9" t="s">
-        <v>797</v>
+        <v>799</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>798</v>
+        <v>800</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>12</v>
@@ -39958,10 +39964,10 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="9" t="s">
-        <v>733</v>
+        <v>735</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>799</v>
+        <v>801</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>13</v>
@@ -39973,10 +39979,10 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="9" t="s">
-        <v>800</v>
+        <v>802</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>801</v>
+        <v>803</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>14</v>
@@ -39988,7 +39994,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="9" t="s">
-        <v>802</v>
+        <v>804</v>
       </c>
       <c r="B17" s="9"/>
       <c r="C17" s="9" t="s">
@@ -40001,10 +40007,10 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="9" t="s">
-        <v>803</v>
+        <v>805</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>804</v>
+        <v>806</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>16</v>
@@ -40016,10 +40022,10 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="9" t="s">
-        <v>805</v>
+        <v>807</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>806</v>
+        <v>808</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>17</v>
@@ -40031,10 +40037,10 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="9" t="s">
-        <v>807</v>
+        <v>809</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>808</v>
+        <v>810</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>18</v>
@@ -40046,10 +40052,10 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="9" t="s">
-        <v>809</v>
+        <v>811</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>810</v>
+        <v>812</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>19</v>
@@ -40061,7 +40067,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="9" t="s">
-        <v>811</v>
+        <v>813</v>
       </c>
       <c r="B22" s="9"/>
       <c r="C22" s="9" t="s">
@@ -40074,10 +40080,10 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="9" t="s">
-        <v>812</v>
+        <v>814</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>813</v>
+        <v>815</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>21</v>
@@ -40089,10 +40095,10 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="9" t="s">
-        <v>814</v>
+        <v>816</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>815</v>
+        <v>817</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>22</v>
@@ -40104,10 +40110,10 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="9" t="s">
-        <v>816</v>
+        <v>818</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>817</v>
+        <v>819</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>23</v>
@@ -40119,10 +40125,10 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="9" t="s">
-        <v>818</v>
+        <v>820</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>819</v>
+        <v>821</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>24</v>
@@ -40134,10 +40140,10 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="9" t="s">
-        <v>820</v>
+        <v>822</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>821</v>
+        <v>823</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>25</v>
@@ -40149,10 +40155,10 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="9" t="s">
-        <v>822</v>
+        <v>824</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>823</v>
+        <v>825</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>26</v>
@@ -40164,10 +40170,10 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="9" t="s">
-        <v>824</v>
+        <v>826</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>825</v>
+        <v>827</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>27</v>
@@ -40179,10 +40185,10 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="9" t="s">
-        <v>826</v>
+        <v>828</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>827</v>
+        <v>829</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>28</v>
@@ -40194,10 +40200,10 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="9" t="s">
-        <v>828</v>
+        <v>830</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>829</v>
+        <v>831</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>29</v>
@@ -40209,10 +40215,10 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="9" t="s">
-        <v>830</v>
+        <v>832</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>831</v>
+        <v>833</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>30</v>
@@ -40224,10 +40230,10 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="9" t="s">
-        <v>832</v>
+        <v>834</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>833</v>
+        <v>835</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>31</v>
@@ -40239,10 +40245,10 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="9" t="s">
-        <v>834</v>
+        <v>836</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>835</v>
+        <v>837</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>32</v>
@@ -40254,10 +40260,10 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="9" t="s">
-        <v>836</v>
+        <v>838</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>837</v>
+        <v>839</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>33</v>
@@ -40269,10 +40275,10 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="9" t="s">
-        <v>838</v>
+        <v>840</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>839</v>
+        <v>841</v>
       </c>
       <c r="C36" s="9" t="s">
         <v>34</v>
@@ -40370,7 +40376,7 @@
   <sheetData>
     <row r="2" spans="1:14" customHeight="1" ht="31.25">
       <c r="B2" s="164" t="s">
-        <v>840</v>
+        <v>842</v>
       </c>
       <c r="C2" s="164"/>
       <c r="D2" s="164"/>
@@ -40380,7 +40386,7 @@
     </row>
     <row r="3" spans="1:14" customHeight="1" ht="28.75">
       <c r="B3" s="163" t="s">
-        <v>841</v>
+        <v>843</v>
       </c>
       <c r="C3" s="163"/>
       <c r="D3" s="163"/>
@@ -40390,7 +40396,7 @@
     </row>
     <row r="4" spans="1:14" customHeight="1" ht="24">
       <c r="B4" s="165" t="s">
-        <v>842</v>
+        <v>844</v>
       </c>
       <c r="C4" s="165"/>
       <c r="D4" s="165"/>
@@ -40400,425 +40406,425 @@
     </row>
     <row r="6" spans="1:14" customHeight="1" ht="20.4">
       <c r="B6" s="1" t="s">
-        <v>843</v>
+        <v>845</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>844</v>
+        <v>846</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>845</v>
+        <v>847</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>846</v>
+        <v>848</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>847</v>
+        <v>849</v>
       </c>
     </row>
     <row r="7" spans="1:14" customHeight="1" ht="22.75">
       <c r="B7" s="1" t="s">
-        <v>848</v>
+        <v>850</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>849</v>
+        <v>851</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>850</v>
+        <v>852</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>851</v>
+        <v>853</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>852</v>
+        <v>854</v>
       </c>
     </row>
     <row r="9" spans="1:14">
       <c r="B9" s="6" t="s">
-        <v>853</v>
+        <v>855</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>854</v>
+        <v>856</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>855</v>
+        <v>857</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>856</v>
+        <v>858</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>857</v>
+        <v>859</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>858</v>
+        <v>860</v>
       </c>
     </row>
     <row r="10" spans="1:14">
       <c r="B10" s="1" t="s">
-        <v>859</v>
+        <v>861</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>860</v>
+        <v>862</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>861</v>
+        <v>863</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>862</v>
+        <v>864</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>863</v>
+        <v>865</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>864</v>
+        <v>866</v>
       </c>
     </row>
     <row r="11" spans="1:14">
       <c r="B11" s="1" t="s">
-        <v>865</v>
+        <v>867</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>866</v>
+        <v>868</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>868</v>
+        <v>870</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>869</v>
+        <v>871</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>870</v>
+        <v>872</v>
       </c>
     </row>
     <row r="12" spans="1:14">
       <c r="B12" s="1" t="s">
-        <v>871</v>
+        <v>873</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>872</v>
+        <v>874</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>873</v>
+        <v>875</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>874</v>
+        <v>876</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>875</v>
+        <v>877</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>876</v>
+        <v>878</v>
       </c>
     </row>
     <row r="13" spans="1:14">
       <c r="B13" s="1" t="s">
-        <v>877</v>
+        <v>879</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>878</v>
+        <v>880</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>880</v>
+        <v>882</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>881</v>
+        <v>883</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>882</v>
+        <v>884</v>
       </c>
     </row>
     <row r="14" spans="1:14">
       <c r="B14" s="1" t="s">
-        <v>883</v>
+        <v>885</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>884</v>
+        <v>886</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>885</v>
+        <v>887</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>886</v>
+        <v>888</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>887</v>
+        <v>889</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>888</v>
+        <v>890</v>
       </c>
     </row>
     <row r="15" spans="1:14">
       <c r="B15" s="1" t="s">
-        <v>889</v>
+        <v>891</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>890</v>
+        <v>892</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>891</v>
+        <v>893</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>892</v>
+        <v>894</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>893</v>
+        <v>895</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>894</v>
+        <v>896</v>
       </c>
     </row>
     <row r="16" spans="1:14">
       <c r="B16" s="1" t="s">
-        <v>895</v>
+        <v>897</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>896</v>
+        <v>898</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>897</v>
+        <v>899</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>898</v>
+        <v>900</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>899</v>
+        <v>901</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>900</v>
+        <v>902</v>
       </c>
     </row>
     <row r="17" spans="1:14">
       <c r="B17" s="1" t="s">
-        <v>901</v>
+        <v>903</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>902</v>
+        <v>904</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>903</v>
+        <v>905</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>904</v>
+        <v>906</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>905</v>
+        <v>907</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>906</v>
+        <v>908</v>
       </c>
     </row>
     <row r="18" spans="1:14">
       <c r="B18" s="1" t="s">
-        <v>907</v>
+        <v>909</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>908</v>
+        <v>910</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>909</v>
+        <v>911</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>910</v>
+        <v>912</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>911</v>
+        <v>913</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>912</v>
+        <v>914</v>
       </c>
     </row>
     <row r="19" spans="1:14">
       <c r="B19" s="1" t="s">
-        <v>913</v>
+        <v>915</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>914</v>
+        <v>916</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>915</v>
+        <v>917</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>916</v>
+        <v>918</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
     </row>
     <row r="20" spans="1:14">
       <c r="B20" s="1" t="s">
-        <v>919</v>
+        <v>921</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>920</v>
+        <v>922</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>921</v>
+        <v>923</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>922</v>
+        <v>924</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>923</v>
+        <v>925</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>924</v>
+        <v>926</v>
       </c>
     </row>
     <row r="21" spans="1:14">
       <c r="B21" s="1" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>926</v>
+        <v>928</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>927</v>
+        <v>929</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>928</v>
+        <v>930</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>929</v>
+        <v>931</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
     </row>
     <row r="22" spans="1:14">
       <c r="B22" s="1" t="s">
-        <v>931</v>
+        <v>933</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>932</v>
+        <v>934</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>933</v>
+        <v>935</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>934</v>
+        <v>936</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>935</v>
+        <v>937</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>936</v>
+        <v>938</v>
       </c>
     </row>
     <row r="23" spans="1:14">
       <c r="B23" s="1" t="s">
-        <v>937</v>
+        <v>939</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>938</v>
+        <v>940</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>939</v>
+        <v>941</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>940</v>
+        <v>942</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>941</v>
+        <v>943</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>942</v>
+        <v>944</v>
       </c>
     </row>
     <row r="24" spans="1:14">
       <c r="B24" s="1" t="s">
-        <v>943</v>
+        <v>945</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>945</v>
+        <v>947</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>946</v>
+        <v>948</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>948</v>
+        <v>950</v>
       </c>
     </row>
     <row r="25" spans="1:14">
       <c r="B25" s="1" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>951</v>
+        <v>953</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>952</v>
+        <v>954</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>953</v>
+        <v>955</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>954</v>
+        <v>956</v>
       </c>
     </row>
     <row r="26" spans="1:14">
       <c r="B26" s="1" t="s">
-        <v>955</v>
+        <v>957</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>958</v>
+        <v>960</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>959</v>
+        <v>961</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>960</v>
+        <v>962</v>
       </c>
     </row>
     <row r="27" spans="1:14">
       <c r="B27" s="1" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>962</v>
+        <v>964</v>
       </c>
       <c r="D27" s="170" t="s">
-        <v>963</v>
+        <v>965</v>
       </c>
       <c r="E27" s="171"/>
       <c r="F27" s="170" t="s">
-        <v>964</v>
+        <v>966</v>
       </c>
       <c r="G27" s="171"/>
     </row>
     <row r="28" spans="1:14">
       <c r="B28" s="1" t="s">
-        <v>965</v>
+        <v>967</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>966</v>
+        <v>968</v>
       </c>
       <c r="D28" s="170" t="s">
-        <v>967</v>
+        <v>969</v>
       </c>
       <c r="E28" s="172"/>
       <c r="F28" s="172"/>
@@ -40826,10 +40832,10 @@
     </row>
     <row r="29" spans="1:14">
       <c r="B29" s="1" t="s">
-        <v>968</v>
+        <v>970</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>969</v>
+        <v>971</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -40838,13 +40844,13 @@
     </row>
     <row r="30" spans="1:14">
       <c r="B30" s="1" t="s">
-        <v>970</v>
+        <v>972</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>971</v>
+        <v>973</v>
       </c>
       <c r="D30" s="170" t="s">
-        <v>972</v>
+        <v>974</v>
       </c>
       <c r="E30" s="172"/>
       <c r="F30" s="172"/>
@@ -40852,13 +40858,13 @@
     </row>
     <row r="31" spans="1:14">
       <c r="B31" s="1" t="s">
-        <v>973</v>
+        <v>975</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="D31" s="170" t="s">
-        <v>975</v>
+        <v>977</v>
       </c>
       <c r="E31" s="172"/>
       <c r="F31" s="172"/>
@@ -40867,11 +40873,11 @@
     <row r="32" spans="1:14" customHeight="1" ht="15"/>
     <row r="33" spans="1:14" customHeight="1" ht="14.5">
       <c r="B33" s="166" t="s">
-        <v>976</v>
+        <v>978</v>
       </c>
       <c r="C33" s="167"/>
       <c r="D33" s="166" t="s">
-        <v>977</v>
+        <v>979</v>
       </c>
       <c r="E33" s="173"/>
       <c r="F33" s="173"/>
@@ -40927,7 +40933,7 @@
     </row>
     <row r="40" spans="1:14">
       <c r="B40" s="154" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
       <c r="C40" s="155"/>
       <c r="D40" s="155"/>
@@ -41001,19 +41007,19 @@
     </row>
     <row r="50" spans="1:14" customHeight="1" ht="23.5">
       <c r="B50" s="3" t="s">
-        <v>979</v>
+        <v>981</v>
       </c>
     </row>
     <row r="51" spans="1:14">
       <c r="B51" s="137" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="C51" s="137" t="s">
-        <v>981</v>
+        <v>983</v>
       </c>
       <c r="D51" s="138"/>
       <c r="E51" s="137" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
       <c r="N51" s="8"/>
     </row>
@@ -41089,95 +41095,95 @@
     </row>
     <row r="67" spans="1:14">
       <c r="B67" s="137" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="C67" s="137" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="E67" s="137" t="s">
-        <v>985</v>
+        <v>987</v>
       </c>
     </row>
     <row r="83" spans="1:14">
       <c r="B83" s="137" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="C83" s="137" t="s">
-        <v>987</v>
+        <v>989</v>
       </c>
       <c r="E83" s="137" t="s">
-        <v>988</v>
+        <v>990</v>
       </c>
     </row>
     <row r="99" spans="1:14" customHeight="1" ht="23.5">
       <c r="B99" s="3" t="s">
-        <v>989</v>
+        <v>991</v>
       </c>
     </row>
     <row r="100" spans="1:14">
       <c r="B100" s="138" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="C100" s="138" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
       <c r="E100" s="138" t="s">
-        <v>992</v>
+        <v>994</v>
       </c>
     </row>
     <row r="116" spans="1:14">
       <c r="B116" s="138" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="C116" s="138" t="s">
-        <v>994</v>
+        <v>996</v>
       </c>
       <c r="E116" s="138" t="s">
-        <v>995</v>
+        <v>997</v>
       </c>
     </row>
     <row r="132" spans="1:14">
       <c r="B132" s="138" t="s">
-        <v>996</v>
+        <v>998</v>
       </c>
       <c r="C132" s="138" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="E132" s="138" t="s">
-        <v>998</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="148" spans="1:14">
       <c r="B148" s="138" t="s">
-        <v>999</v>
+        <v>1001</v>
       </c>
       <c r="C148" s="138" t="s">
-        <v>1000</v>
+        <v>1002</v>
       </c>
       <c r="E148" s="138" t="s">
-        <v>1001</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="164" spans="1:14">
       <c r="B164" s="138" t="s">
-        <v>1002</v>
+        <v>1004</v>
       </c>
       <c r="C164" s="138" t="s">
-        <v>1003</v>
+        <v>1005</v>
       </c>
       <c r="E164" s="138" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="179" spans="1:14">
       <c r="B179" s="138" t="s">
-        <v>1005</v>
+        <v>1007</v>
       </c>
       <c r="C179" s="138" t="s">
-        <v>1006</v>
+        <v>1008</v>
       </c>
       <c r="E179" s="138" t="s">
-        <v>1007</v>
+        <v>1009</v>
       </c>
     </row>
   </sheetData>

</xml_diff>